<commit_message>
Refactoring - add Rodent circovirus-1 Rep
</commit_message>
<xml_diff>
--- a/tabular/genus/circo-refseqs-side-data.xlsx
+++ b/tabular/genus/circo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/CRESS-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70508013-D0F8-ED46-A6EE-DA7CD82EDEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1780CE79-8624-C744-9A99-BA816E38B341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
   <si>
     <t>PCV-1</t>
   </si>
@@ -292,6 +292,21 @@
   </si>
   <si>
     <t>Circoviridae</t>
+  </si>
+  <si>
+    <t>KY370034</t>
+  </si>
+  <si>
+    <t>RodentCV-1</t>
+  </si>
+  <si>
+    <t>Rodent circovirus 1</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>Neodon clarkei</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD176"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1985,32 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="22" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:8" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>

</xml_diff>